<commit_message>
Update of files examples/Cylinder/probes_pos.csv and examples/Cylinder/probes_pos.xlsx
</commit_message>
<xml_diff>
--- a/examples/Cylinder/probes_pos.xlsx
+++ b/examples/Cylinder/probes_pos.xlsx
@@ -146,13 +146,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.07"/>
@@ -226,19 +226,19 @@
         <v>9</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false">(G5-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G5)*$D$2/($D$4-1)</f>
         <v>0</v>
       </c>
       <c r="E5" s="0" t="n">
-        <f aca="false">INT(B5*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B5*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F5" s="0" t="n">
-        <f aca="false">INT(C5*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C5*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -252,19 +252,19 @@
         <v>9</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">(G6-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G6)*$D$2/($D$4-1)</f>
         <v>0.4</v>
       </c>
       <c r="E6" s="0" t="n">
-        <f aca="false">INT(B6*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B6*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F6" s="0" t="n">
-        <f aca="false">INT(C6*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C6*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,19 +278,19 @@
         <v>9</v>
       </c>
       <c r="D7" s="0" t="n">
-        <f aca="false">(G7-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G7)*$D$2/($D$4-1)</f>
         <v>0.8</v>
       </c>
       <c r="E7" s="0" t="n">
-        <f aca="false">INT(B7*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B7*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F7" s="0" t="n">
-        <f aca="false">INT(C7*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C7*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,19 +304,19 @@
         <v>9</v>
       </c>
       <c r="D8" s="0" t="n">
-        <f aca="false">(G8-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G8)*$D$2/($D$4-1)</f>
         <v>1.2</v>
       </c>
       <c r="E8" s="0" t="n">
-        <f aca="false">INT(B8*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B8*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F8" s="0" t="n">
-        <f aca="false">INT(C8*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C8*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -330,19 +330,19 @@
         <v>9</v>
       </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">(G9-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G9)*$D$2/($D$4-1)</f>
         <v>1.6</v>
       </c>
       <c r="E9" s="0" t="n">
-        <f aca="false">INT(B9*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B9*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F9" s="0" t="n">
-        <f aca="false">INT(C9*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C9*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,19 +356,19 @@
         <v>9</v>
       </c>
       <c r="D10" s="0" t="n">
-        <f aca="false">(G10-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G10)*$D$2/($D$4-1)</f>
         <v>2</v>
       </c>
       <c r="E10" s="0" t="n">
-        <f aca="false">INT(B10*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B10*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F10" s="0" t="n">
-        <f aca="false">INT(C10*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C10*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -382,19 +382,19 @@
         <v>9</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">(G11-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G11)*$D$2/($D$4-1)</f>
         <v>2.4</v>
       </c>
       <c r="E11" s="0" t="n">
-        <f aca="false">INT(B11*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B11*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F11" s="0" t="n">
-        <f aca="false">INT(C11*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C11*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,19 +408,19 @@
         <v>9</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">(G12-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G12)*$D$2/($D$4-1)</f>
         <v>2.8</v>
       </c>
       <c r="E12" s="0" t="n">
-        <f aca="false">INT(B12*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B12*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F12" s="0" t="n">
-        <f aca="false">INT(C12*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C12*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,19 +434,19 @@
         <v>9</v>
       </c>
       <c r="D13" s="0" t="n">
-        <f aca="false">(G13-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G13)*$D$2/($D$4-1)</f>
         <v>3.2</v>
       </c>
       <c r="E13" s="0" t="n">
-        <f aca="false">INT(B13*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B13*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F13" s="0" t="n">
-        <f aca="false">INT(C13*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C13*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,19 +460,19 @@
         <v>9</v>
       </c>
       <c r="D14" s="0" t="n">
-        <f aca="false">(G14-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G14)*$D$2/($D$4-1)</f>
         <v>3.6</v>
       </c>
       <c r="E14" s="0" t="n">
-        <f aca="false">INT(B14*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B14*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F14" s="0" t="n">
-        <f aca="false">INT(C14*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C14*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -486,19 +486,19 @@
         <v>9</v>
       </c>
       <c r="D15" s="0" t="n">
-        <f aca="false">(G15-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G15)*$D$2/($D$4-1)</f>
         <v>4</v>
       </c>
       <c r="E15" s="0" t="n">
-        <f aca="false">INT(B15*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B15*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F15" s="0" t="n">
-        <f aca="false">INT(C15*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C15*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,19 +512,19 @@
         <v>9</v>
       </c>
       <c r="D16" s="0" t="n">
-        <f aca="false">(G16-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G16)*$D$2/($D$4-1)</f>
         <v>4.4</v>
       </c>
       <c r="E16" s="0" t="n">
-        <f aca="false">INT(B16*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B16*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F16" s="0" t="n">
-        <f aca="false">INT(C16*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C16*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,19 +538,19 @@
         <v>9</v>
       </c>
       <c r="D17" s="0" t="n">
-        <f aca="false">(G17-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G17)*$D$2/($D$4-1)</f>
         <v>4.8</v>
       </c>
       <c r="E17" s="0" t="n">
-        <f aca="false">INT(B17*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B17*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F17" s="0" t="n">
-        <f aca="false">INT(C17*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C17*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,19 +564,19 @@
         <v>9</v>
       </c>
       <c r="D18" s="0" t="n">
-        <f aca="false">(G18-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G18)*$D$2/($D$4-1)</f>
         <v>5.2</v>
       </c>
       <c r="E18" s="0" t="n">
-        <f aca="false">INT(B18*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B18*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F18" s="0" t="n">
-        <f aca="false">INT(C18*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C18*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,19 +590,19 @@
         <v>9</v>
       </c>
       <c r="D19" s="0" t="n">
-        <f aca="false">(G19-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G19)*$D$2/($D$4-1)</f>
         <v>5.6</v>
       </c>
       <c r="E19" s="0" t="n">
-        <f aca="false">INT(B19*$B$4/$B$2)</f>
-        <v>36</v>
+        <f aca="false">INT(B19*$B$4/$B$2)-1</f>
+        <v>35</v>
       </c>
       <c r="F19" s="0" t="n">
-        <f aca="false">INT(C19*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C19*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,25 +610,25 @@
         <v>16</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>8.75</v>
+        <v>9</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>9.65</v>
+        <v>9</v>
       </c>
       <c r="D20" s="0" t="n">
-        <f aca="false">(G20-1)*$D$2/($D$4-1)</f>
-        <v>0</v>
+        <f aca="false">(G20)*$D$2/($D$4-1)</f>
+        <v>6</v>
       </c>
       <c r="E20" s="0" t="n">
-        <f aca="false">INT(B20*$B$4/$B$2)</f>
+        <f aca="false">INT(B20*$B$4/$B$2)-1</f>
         <v>35</v>
       </c>
       <c r="F20" s="0" t="n">
-        <f aca="false">INT(C20*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C20*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,19 +642,19 @@
         <v>9.65</v>
       </c>
       <c r="D21" s="0" t="n">
-        <f aca="false">(G21-1)*$D$2/($D$4-1)</f>
-        <v>0.4</v>
+        <f aca="false">(G21)*$D$2/($D$4-1)</f>
+        <v>0</v>
       </c>
       <c r="E21" s="0" t="n">
-        <f aca="false">INT(B21*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B21*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F21" s="0" t="n">
-        <f aca="false">INT(C21*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C21*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,19 +668,19 @@
         <v>9.65</v>
       </c>
       <c r="D22" s="0" t="n">
-        <f aca="false">(G22-1)*$D$2/($D$4-1)</f>
-        <v>0.8</v>
+        <f aca="false">(G22)*$D$2/($D$4-1)</f>
+        <v>0.4</v>
       </c>
       <c r="E22" s="0" t="n">
-        <f aca="false">INT(B22*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B22*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F22" s="0" t="n">
-        <f aca="false">INT(C22*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C22*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,19 +694,19 @@
         <v>9.65</v>
       </c>
       <c r="D23" s="0" t="n">
-        <f aca="false">(G23-1)*$D$2/($D$4-1)</f>
-        <v>1.2</v>
+        <f aca="false">(G23)*$D$2/($D$4-1)</f>
+        <v>0.8</v>
       </c>
       <c r="E23" s="0" t="n">
-        <f aca="false">INT(B23*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B23*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F23" s="0" t="n">
-        <f aca="false">INT(C23*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C23*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -720,19 +720,19 @@
         <v>9.65</v>
       </c>
       <c r="D24" s="0" t="n">
-        <f aca="false">(G24-1)*$D$2/($D$4-1)</f>
-        <v>1.6</v>
+        <f aca="false">(G24)*$D$2/($D$4-1)</f>
+        <v>1.2</v>
       </c>
       <c r="E24" s="0" t="n">
-        <f aca="false">INT(B24*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B24*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F24" s="0" t="n">
-        <f aca="false">INT(C24*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C24*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,19 +746,19 @@
         <v>9.65</v>
       </c>
       <c r="D25" s="0" t="n">
-        <f aca="false">(G25-1)*$D$2/($D$4-1)</f>
-        <v>2</v>
+        <f aca="false">(G25)*$D$2/($D$4-1)</f>
+        <v>1.6</v>
       </c>
       <c r="E25" s="0" t="n">
-        <f aca="false">INT(B25*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B25*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F25" s="0" t="n">
-        <f aca="false">INT(C25*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C25*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,19 +772,19 @@
         <v>9.65</v>
       </c>
       <c r="D26" s="0" t="n">
-        <f aca="false">(G26-1)*$D$2/($D$4-1)</f>
-        <v>2.4</v>
+        <f aca="false">(G26)*$D$2/($D$4-1)</f>
+        <v>2</v>
       </c>
       <c r="E26" s="0" t="n">
-        <f aca="false">INT(B26*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B26*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F26" s="0" t="n">
-        <f aca="false">INT(C26*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C26*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,19 +798,19 @@
         <v>9.65</v>
       </c>
       <c r="D27" s="0" t="n">
-        <f aca="false">(G27-1)*$D$2/($D$4-1)</f>
-        <v>2.8</v>
+        <f aca="false">(G27)*$D$2/($D$4-1)</f>
+        <v>2.4</v>
       </c>
       <c r="E27" s="0" t="n">
-        <f aca="false">INT(B27*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B27*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F27" s="0" t="n">
-        <f aca="false">INT(C27*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C27*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,19 +824,19 @@
         <v>9.65</v>
       </c>
       <c r="D28" s="0" t="n">
-        <f aca="false">(G28-1)*$D$2/($D$4-1)</f>
-        <v>3.2</v>
+        <f aca="false">(G28)*$D$2/($D$4-1)</f>
+        <v>2.8</v>
       </c>
       <c r="E28" s="0" t="n">
-        <f aca="false">INT(B28*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B28*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F28" s="0" t="n">
-        <f aca="false">INT(C28*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C28*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,19 +850,19 @@
         <v>9.65</v>
       </c>
       <c r="D29" s="0" t="n">
-        <f aca="false">(G29-1)*$D$2/($D$4-1)</f>
-        <v>3.6</v>
+        <f aca="false">(G29)*$D$2/($D$4-1)</f>
+        <v>3.2</v>
       </c>
       <c r="E29" s="0" t="n">
-        <f aca="false">INT(B29*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B29*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F29" s="0" t="n">
-        <f aca="false">INT(C29*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C29*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,19 +876,19 @@
         <v>9.65</v>
       </c>
       <c r="D30" s="0" t="n">
-        <f aca="false">(G30-1)*$D$2/($D$4-1)</f>
-        <v>4</v>
+        <f aca="false">(G30)*$D$2/($D$4-1)</f>
+        <v>3.6</v>
       </c>
       <c r="E30" s="0" t="n">
-        <f aca="false">INT(B30*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B30*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F30" s="0" t="n">
-        <f aca="false">INT(C30*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C30*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,19 +902,19 @@
         <v>9.65</v>
       </c>
       <c r="D31" s="0" t="n">
-        <f aca="false">(G31-1)*$D$2/($D$4-1)</f>
-        <v>4.4</v>
+        <f aca="false">(G31)*$D$2/($D$4-1)</f>
+        <v>4</v>
       </c>
       <c r="E31" s="0" t="n">
-        <f aca="false">INT(B31*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B31*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F31" s="0" t="n">
-        <f aca="false">INT(C31*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C31*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,19 +928,19 @@
         <v>9.65</v>
       </c>
       <c r="D32" s="0" t="n">
-        <f aca="false">(G32-1)*$D$2/($D$4-1)</f>
-        <v>4.8</v>
+        <f aca="false">(G32)*$D$2/($D$4-1)</f>
+        <v>4.4</v>
       </c>
       <c r="E32" s="0" t="n">
-        <f aca="false">INT(B32*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B32*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F32" s="0" t="n">
-        <f aca="false">INT(C32*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C32*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -954,19 +954,19 @@
         <v>9.65</v>
       </c>
       <c r="D33" s="0" t="n">
-        <f aca="false">(G33-1)*$D$2/($D$4-1)</f>
-        <v>5.2</v>
+        <f aca="false">(G33)*$D$2/($D$4-1)</f>
+        <v>4.8</v>
       </c>
       <c r="E33" s="0" t="n">
-        <f aca="false">INT(B33*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B33*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F33" s="0" t="n">
-        <f aca="false">INT(C33*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C33*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,19 +980,19 @@
         <v>9.65</v>
       </c>
       <c r="D34" s="0" t="n">
-        <f aca="false">(G34-1)*$D$2/($D$4-1)</f>
-        <v>5.6</v>
+        <f aca="false">(G34)*$D$2/($D$4-1)</f>
+        <v>5.2</v>
       </c>
       <c r="E34" s="0" t="n">
-        <f aca="false">INT(B34*$B$4/$B$2)</f>
-        <v>35</v>
+        <f aca="false">INT(B34*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F34" s="0" t="n">
-        <f aca="false">INT(C34*$C$4/$C$2)</f>
-        <v>32</v>
+        <f aca="false">INT(C34*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,25 +1000,25 @@
         <v>31</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>11.5</v>
+        <v>8.75</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>9</v>
+        <v>9.65</v>
       </c>
       <c r="D35" s="0" t="n">
-        <f aca="false">(G35-1)*$D$2/($D$4-1)</f>
-        <v>0</v>
+        <f aca="false">(G35)*$D$2/($D$4-1)</f>
+        <v>5.6</v>
       </c>
       <c r="E35" s="0" t="n">
-        <f aca="false">INT(B35*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B35*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F35" s="0" t="n">
-        <f aca="false">INT(C35*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C35*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G35" s="0" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,25 +1026,25 @@
         <v>32</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>11.5</v>
+        <v>8.75</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>9</v>
+        <v>9.65</v>
       </c>
       <c r="D36" s="0" t="n">
-        <f aca="false">(G36-1)*$D$2/($D$4-1)</f>
-        <v>0.4</v>
+        <f aca="false">(G36)*$D$2/($D$4-1)</f>
+        <v>6</v>
       </c>
       <c r="E36" s="0" t="n">
-        <f aca="false">INT(B36*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B36*$B$4/$B$2)-1</f>
+        <v>34</v>
       </c>
       <c r="F36" s="0" t="n">
-        <f aca="false">INT(C36*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C36*$C$4/$C$2)-1</f>
+        <v>31</v>
       </c>
       <c r="G36" s="0" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,19 +1058,19 @@
         <v>9</v>
       </c>
       <c r="D37" s="0" t="n">
-        <f aca="false">(G37-1)*$D$2/($D$4-1)</f>
-        <v>0.8</v>
+        <f aca="false">(G37)*$D$2/($D$4-1)</f>
+        <v>0</v>
       </c>
       <c r="E37" s="0" t="n">
-        <f aca="false">INT(B37*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B37*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F37" s="0" t="n">
-        <f aca="false">INT(C37*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C37*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,19 +1084,19 @@
         <v>9</v>
       </c>
       <c r="D38" s="0" t="n">
-        <f aca="false">(G38-1)*$D$2/($D$4-1)</f>
-        <v>1.2</v>
+        <f aca="false">(G38)*$D$2/($D$4-1)</f>
+        <v>0.4</v>
       </c>
       <c r="E38" s="0" t="n">
-        <f aca="false">INT(B38*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B38*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F38" s="0" t="n">
-        <f aca="false">INT(C38*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C38*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G38" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,19 +1110,19 @@
         <v>9</v>
       </c>
       <c r="D39" s="0" t="n">
-        <f aca="false">(G39-1)*$D$2/($D$4-1)</f>
-        <v>1.6</v>
+        <f aca="false">(G39)*$D$2/($D$4-1)</f>
+        <v>1.2</v>
       </c>
       <c r="E39" s="0" t="n">
-        <f aca="false">INT(B39*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B39*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F39" s="0" t="n">
-        <f aca="false">INT(C39*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C39*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G39" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,19 +1136,19 @@
         <v>9</v>
       </c>
       <c r="D40" s="0" t="n">
-        <f aca="false">(G40-1)*$D$2/($D$4-1)</f>
-        <v>2</v>
+        <f aca="false">(G40)*$D$2/($D$4-1)</f>
+        <v>1.6</v>
       </c>
       <c r="E40" s="0" t="n">
-        <f aca="false">INT(B40*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B40*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F40" s="0" t="n">
-        <f aca="false">INT(C40*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C40*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,19 +1162,19 @@
         <v>9</v>
       </c>
       <c r="D41" s="0" t="n">
-        <f aca="false">(G41-1)*$D$2/($D$4-1)</f>
-        <v>2.4</v>
+        <f aca="false">(G41)*$D$2/($D$4-1)</f>
+        <v>2</v>
       </c>
       <c r="E41" s="0" t="n">
-        <f aca="false">INT(B41*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B41*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F41" s="0" t="n">
-        <f aca="false">INT(C41*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C41*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G41" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,19 +1188,19 @@
         <v>9</v>
       </c>
       <c r="D42" s="0" t="n">
-        <f aca="false">(G42-1)*$D$2/($D$4-1)</f>
-        <v>2.8</v>
+        <f aca="false">(G42)*$D$2/($D$4-1)</f>
+        <v>2.4</v>
       </c>
       <c r="E42" s="0" t="n">
-        <f aca="false">INT(B42*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B42*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F42" s="0" t="n">
-        <f aca="false">INT(C42*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C42*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G42" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,19 +1214,19 @@
         <v>9</v>
       </c>
       <c r="D43" s="0" t="n">
-        <f aca="false">(G43-1)*$D$2/($D$4-1)</f>
-        <v>3.2</v>
+        <f aca="false">(G43)*$D$2/($D$4-1)</f>
+        <v>2.8</v>
       </c>
       <c r="E43" s="0" t="n">
-        <f aca="false">INT(B43*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B43*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F43" s="0" t="n">
-        <f aca="false">INT(C43*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C43*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1240,19 +1240,19 @@
         <v>9</v>
       </c>
       <c r="D44" s="0" t="n">
-        <f aca="false">(G44-1)*$D$2/($D$4-1)</f>
-        <v>3.6</v>
+        <f aca="false">(G44)*$D$2/($D$4-1)</f>
+        <v>3.2</v>
       </c>
       <c r="E44" s="0" t="n">
-        <f aca="false">INT(B44*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B44*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F44" s="0" t="n">
-        <f aca="false">INT(C44*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C44*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,19 +1266,19 @@
         <v>9</v>
       </c>
       <c r="D45" s="0" t="n">
-        <f aca="false">(G45-1)*$D$2/($D$4-1)</f>
-        <v>4</v>
+        <f aca="false">(G45)*$D$2/($D$4-1)</f>
+        <v>3.6</v>
       </c>
       <c r="E45" s="0" t="n">
-        <f aca="false">INT(B45*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B45*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F45" s="0" t="n">
-        <f aca="false">INT(C45*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C45*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,19 +1292,19 @@
         <v>9</v>
       </c>
       <c r="D46" s="0" t="n">
-        <f aca="false">(G46-1)*$D$2/($D$4-1)</f>
-        <v>4.4</v>
+        <f aca="false">(G46)*$D$2/($D$4-1)</f>
+        <v>4</v>
       </c>
       <c r="E46" s="0" t="n">
-        <f aca="false">INT(B46*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B46*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F46" s="0" t="n">
-        <f aca="false">INT(C46*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C46*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,19 +1318,19 @@
         <v>9</v>
       </c>
       <c r="D47" s="0" t="n">
-        <f aca="false">(G47-1)*$D$2/($D$4-1)</f>
-        <v>4.8</v>
+        <f aca="false">(G47)*$D$2/($D$4-1)</f>
+        <v>4.4</v>
       </c>
       <c r="E47" s="0" t="n">
-        <f aca="false">INT(B47*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B47*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F47" s="0" t="n">
-        <f aca="false">INT(C47*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C47*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,19 +1344,19 @@
         <v>9</v>
       </c>
       <c r="D48" s="0" t="n">
-        <f aca="false">(G48-1)*$D$2/($D$4-1)</f>
-        <v>5.2</v>
+        <f aca="false">(G48)*$D$2/($D$4-1)</f>
+        <v>4.8</v>
       </c>
       <c r="E48" s="0" t="n">
-        <f aca="false">INT(B48*$B$4/$B$2)</f>
-        <v>46</v>
+        <f aca="false">INT(B48*$B$4/$B$2)-1</f>
+        <v>45</v>
       </c>
       <c r="F48" s="0" t="n">
-        <f aca="false">INT(C48*$C$4/$C$2)</f>
-        <v>30</v>
+        <f aca="false">INT(C48*$C$4/$C$2)-1</f>
+        <v>29</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,18 +1370,70 @@
         <v>9</v>
       </c>
       <c r="D49" s="0" t="n">
-        <f aca="false">(G49-1)*$D$2/($D$4-1)</f>
+        <f aca="false">(G49)*$D$2/($D$4-1)</f>
+        <v>5.2</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <f aca="false">INT(B49*$B$4/$B$2)-1</f>
+        <v>45</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <f aca="false">INT(C49*$C$4/$C$2)-1</f>
+        <v>29</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <f aca="false">(G50)*$D$2/($D$4-1)</f>
         <v>5.6</v>
       </c>
-      <c r="E49" s="0" t="n">
-        <f aca="false">INT(B49*$B$4/$B$2)</f>
-        <v>46</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <f aca="false">INT(C49*$C$4/$C$2)</f>
-        <v>30</v>
-      </c>
-      <c r="G49" s="0" t="n">
+      <c r="E50" s="0" t="n">
+        <f aca="false">INT(B50*$B$4/$B$2)-1</f>
+        <v>45</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <f aca="false">INT(C50*$C$4/$C$2)-1</f>
+        <v>29</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <f aca="false">(G51)*$D$2/($D$4-1)</f>
+        <v>6</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <f aca="false">INT(B51*$B$4/$B$2)-1</f>
+        <v>45</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <f aca="false">INT(C51*$C$4/$C$2)-1</f>
+        <v>29</v>
+      </c>
+      <c r="G51" s="0" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>